<commit_message>
draft extensive note; fix category names;introduce new coef plot
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output REGIONS 2022.xlsx
+++ b/OUTPUT/DATA/Regression output REGIONS 2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -95,397 +95,469 @@
     <t xml:space="preserve">Main simple (**)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7784 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.7685, 0.7884]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.09719 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1285, -0.0659]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.06036 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1089, -0.01184]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1603 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2102, -0.1103]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">          </t>
+    <t xml:space="preserve">0.78 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.77, 0.79]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.097 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.13, -0.066]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.06 *   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.012]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.21, -0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
   </si>
   <si>
     <t xml:space="preserve">** + age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7105 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.6894, 0.7317]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1089 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1396, -0.07832]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.09853, -0.001033]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1563 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2052, -0.1073]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.6571 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.7252, -0.589]     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2025 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.295, -0.1101]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1085 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.0848, 0.1323]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.08341 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.05272, 0.1141]    </t>
+    <t xml:space="preserve">0.71 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.69, 0.73]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.078]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.099, -0.001]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.66 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.73, -0.59]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.2 ***  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.3, -0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.085, 0.13]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.083 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.053, 0.11]    </t>
   </si>
   <si>
     <t xml:space="preserve">** + eth</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7999 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.7897, 0.8101]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.04309 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.07441, -0.01177]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.08069, 0.01075]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1029 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1527, -0.0531]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1655 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.193, -0.138]    </t>
+    <t xml:space="preserve">0.8 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.79, 0.81]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.043 * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.074, -0.012]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.081, 0.011]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.15, -0.053]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.17 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.19, -0.14]   </t>
   </si>
   <si>
     <t xml:space="preserve">** + child age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8094 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.7981, 0.8207]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.09478 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1257, -0.06387]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1057, -0.008483]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1543 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2038, -0.1047]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.08024 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.104, -0.05648]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.08135 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1099, -0.05279]   </t>
+    <t xml:space="preserve">0.81 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.8, 0.82]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.095 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.13, -0.064]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.0085]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.15 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.2, -0.1]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.08 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.056]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.081 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.053]   </t>
   </si>
   <si>
     <t xml:space="preserve">** + famtype</t>
   </si>
   <si>
-    <t xml:space="preserve">0.6788 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.6564, 0.7013]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.09843 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1297, -0.06716]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1025, -0.005716]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1531 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2025, -0.1038]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1248 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.1006, 0.1489]    </t>
+    <t xml:space="preserve">0.68 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.66, 0.7]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.098 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.13, -0.067]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.0057]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.12 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.1, 0.15]    </t>
   </si>
   <si>
     <t xml:space="preserve">** + religion</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7918 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.7784, 0.8053]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0459 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.07669, -0.01511]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.06124, 0.02752]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.09853 **</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1484, -0.04867]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.01164, 0.02568]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1625 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.283, -0.04194]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.09492, 0.03597]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.03478, 0.1842]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.3284 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.3733, -0.2834]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1725, 0.05648]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1753, -0.007276] </t>
+    <t xml:space="preserve">0.79 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.78, 0.81]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.046 * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.077, -0.015]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.061, 0.028]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.099 **</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.15, -0.049]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.012, 0.026]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.28, -0.042]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.095, 0.036]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.035, 0.18]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.33 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.37, -0.28]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.17, 0.056]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.18, -0.0073] </t>
   </si>
   <si>
     <t xml:space="preserve">** + disability</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8305 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.8204, 0.8406]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1088 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1396, -0.07788]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.09214, -0.0002278]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1619 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2117, -0.1121]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2436 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2684, -0.2189]   </t>
+    <t xml:space="preserve">0.83 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.82, 0.84]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.078]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.092, -0.00023]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.21, -0.11]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.24 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.27, -0.22]   </t>
   </si>
   <si>
     <t xml:space="preserve">** + num_children</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8037 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.7895, 0.8178]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0997 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1317, -0.06771]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.09926, -0.001565] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1205 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1705, -0.07052]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.01186, 0.0261]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.3479 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.4084, -0.2874]   </t>
+    <t xml:space="preserve">0.8 ***  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.79, 0.82]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.093 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.12, -0.062]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.0061]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.14 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.18, -0.089]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.012, 0.026]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.23, -0.17]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">** + age + child age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.73 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.71, 0.76]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.076]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.099, -0.0011]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.29, -0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.095 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.069, 0.12]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06 **  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.025, 0.094]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.051, 0.0032]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.05 **  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.079, -0.021]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">** + eth + religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.79 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.78, 0.81]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.066, -0.0035]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.057, 0.031]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.087 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.037]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.073 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.038]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.0056, 0.032]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.22, 0.023]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.037, 0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.032, 0.18]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.27 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.32, -0.22]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, 0.12]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.16, 0.0066]  </t>
   </si>
   <si>
     <t xml:space="preserve">full</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8004 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.7681, 0.8328]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.05575 ** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.08695, -0.02455]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.028, 0.05676]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.09474, 0.0005007] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.7489 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.8062, -0.6915]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1955 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.284, -0.1069]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07651 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.05064, 0.1024]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.0172, 0.05088]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.06834 ** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1033, -0.03334]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.03989, 0.01287]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.03423 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.0623, -0.006168]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07582 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [0.05179, 0.09984]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.04029, -0.003201]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1973 **  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.319, -0.07568]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1148, 0.02551]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.06117, 0.1362]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2542 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.312, -0.1964]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2268, 0.03425]   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.1635, -0.004396]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2271 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.2525, -0.2016]    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.03656, 0.000109]  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2914 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI [-0.3494, -0.2334]    </t>
+    <t xml:space="preserve">[0.75, 0.82]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.049 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.079, -0.019]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.025, 0.057]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.015]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.73 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.78, -0.68]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.19 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.27, -0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.088 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.063, 0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.012, 0.054]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.036]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.051, -0.00081] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.041 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.068, -0.014]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.085 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.062, 0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.031, 0.005]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.19 **  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.31, -0.069]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.12, 0.022]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.053, 0.14]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.25 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.3, -0.2]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.18, 0.066]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, 0.0094]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.22 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.25, -0.2]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.039, -0.0021]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.18 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.21, -0.15]    </t>
   </si>
 </sst>
 </file>
@@ -943,6 +1015,8 @@
     <col min="8" max="8" width="10.71" hidden="0" customWidth="1"/>
     <col min="9" max="9" width="10.71" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="10.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="10.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="10.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="NA" customHeight="1">
@@ -956,25 +1030,31 @@
         <v>36</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -988,25 +1068,31 @@
         <v>37</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
@@ -1020,25 +1106,31 @@
         <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="4" ht="NA" customHeight="1">
@@ -1052,25 +1144,31 @@
         <v>39</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>126</v>
+        <v>39</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>-0.035</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
@@ -1084,25 +1182,31 @@
         <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
@@ -1113,28 +1217,34 @@
         <v>31</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>-0.04978</v>
+        <v>-0.05</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>-0.03497</v>
+        <v>-0.035</v>
       </c>
       <c r="E6" s="7" t="n">
-        <v>-0.05708</v>
+        <v>-0.057</v>
       </c>
       <c r="F6" s="7" t="n">
-        <v>-0.05409</v>
+        <v>-0.054</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>-0.01686</v>
+        <v>-0.017</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>-0.04618</v>
+        <v>-0.046</v>
       </c>
       <c r="I6" s="7" t="n">
-        <v>-0.05041</v>
+        <v>-0.053</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>0.01438</v>
+        <v>-0.05</v>
+      </c>
+      <c r="K6" s="7" t="n">
+        <v>-0.013</v>
+      </c>
+      <c r="L6" s="7" t="n">
+        <v>0.016</v>
       </c>
     </row>
     <row r="7" ht="NA" customHeight="1">
@@ -1148,25 +1258,31 @@
         <v>41</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
@@ -1177,28 +1293,34 @@
         <v>33</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="J8" s="7" t="n">
-        <v>-0.04712</v>
+        <v>114</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -1209,28 +1331,34 @@
         <v>34</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>129</v>
+        <v>68</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
@@ -1241,10 +1369,10 @@
         <v>35</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>35</v>
@@ -1253,16 +1381,22 @@
         <v>35</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>130</v>
+        <v>42</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -1273,10 +1407,10 @@
         <v>35</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>35</v>
@@ -1285,16 +1419,22 @@
         <v>35</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>131</v>
+        <v>43</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
@@ -1305,10 +1445,10 @@
         <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>35</v>
@@ -1317,16 +1457,22 @@
         <v>35</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>132</v>
+        <v>44</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
@@ -1337,10 +1483,10 @@
         <v>35</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>35</v>
@@ -1349,16 +1495,22 @@
         <v>35</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>133</v>
+        <v>123</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -1369,10 +1521,10 @@
         <v>35</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>35</v>
@@ -1381,16 +1533,22 @@
         <v>35</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
@@ -1401,10 +1559,10 @@
         <v>35</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>35</v>
@@ -1413,16 +1571,22 @@
         <v>35</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1433,10 +1597,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>35</v>
@@ -1445,16 +1609,22 @@
         <v>35</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="7" t="n">
-        <v>0.01684</v>
+        <v>35</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="7" t="n">
+        <v>0.021</v>
       </c>
     </row>
     <row r="17" ht="NA" customHeight="1">
@@ -1465,10 +1635,10 @@
         <v>35</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>35</v>
@@ -1477,16 +1647,22 @@
         <v>35</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>136</v>
+        <v>127</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="18" ht="NA" customHeight="1">
@@ -1500,7 +1676,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>35</v>
@@ -1509,16 +1685,22 @@
         <v>35</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>137</v>
+        <v>35</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="19" ht="NA" customHeight="1">
@@ -1532,7 +1714,7 @@
         <v>35</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>35</v>
@@ -1541,16 +1723,22 @@
         <v>35</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>138</v>
+        <v>35</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="20" ht="NA" customHeight="1">
@@ -1564,25 +1752,31 @@
         <v>35</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J20" s="7" t="n">
-        <v>-0.01351</v>
+        <v>-0.024</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="7" t="n">
+        <v>-0.026</v>
       </c>
     </row>
     <row r="21" ht="NA" customHeight="1">
@@ -1596,25 +1790,31 @@
         <v>35</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>139</v>
+        <v>128</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
@@ -1628,25 +1828,31 @@
         <v>35</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>140</v>
+        <v>129</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
@@ -1660,25 +1866,31 @@
         <v>35</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>141</v>
+        <v>130</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
@@ -1692,25 +1904,31 @@
         <v>35</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>35</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>142</v>
+        <v>35</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="25" ht="NA" customHeight="1">
@@ -1724,25 +1942,31 @@
         <v>35</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>143</v>
+        <v>35</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="26" ht="NA" customHeight="1">
@@ -1756,7 +1980,7 @@
         <v>35</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>35</v>
@@ -1765,16 +1989,22 @@
         <v>35</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>0.007019</v>
+        <v>0.007</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26" s="7" t="n">
-        <v>-0.02175</v>
+        <v>35</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="7" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="L26" s="7" t="n">
+        <v>-0.013</v>
       </c>
     </row>
     <row r="27" ht="NA" customHeight="1">
@@ -1788,7 +2018,7 @@
         <v>35</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>35</v>
@@ -1797,16 +2027,22 @@
         <v>35</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>144</v>
+        <v>35</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="28" ht="NA" customHeight="1">
@@ -1820,7 +2056,7 @@
         <v>35</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>35</v>
@@ -1829,16 +2065,22 @@
         <v>35</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>145</v>
+        <v>35</v>
+      </c>
+      <c r="K28" s="7" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
@@ -1852,7 +2094,7 @@
         <v>35</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>35</v>
@@ -1861,16 +2103,22 @@
         <v>35</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>146</v>
+        <v>35</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="30" ht="NA" customHeight="1">
@@ -1884,7 +2132,7 @@
         <v>35</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>35</v>
@@ -1893,16 +2141,22 @@
         <v>35</v>
       </c>
       <c r="G30" s="7" t="n">
-        <v>-0.02947</v>
+        <v>-0.029</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" s="7" t="n">
-        <v>-0.04466</v>
+        <v>35</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" s="7" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="L30" s="7" t="n">
+        <v>-0.047</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
@@ -1916,7 +2170,7 @@
         <v>35</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>35</v>
@@ -1925,16 +2179,22 @@
         <v>35</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>147</v>
+        <v>35</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
@@ -1948,7 +2208,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>35</v>
@@ -1957,16 +2217,22 @@
         <v>35</v>
       </c>
       <c r="G32" s="7" t="n">
-        <v>0.07473</v>
+        <v>0.075</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J32" s="7" t="n">
-        <v>0.0375</v>
+        <v>35</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" s="7" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="L32" s="7" t="n">
+        <v>0.042</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
@@ -1980,7 +2246,7 @@
         <v>35</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>35</v>
@@ -1989,16 +2255,22 @@
         <v>35</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>148</v>
+        <v>35</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">
@@ -2012,7 +2284,7 @@
         <v>35</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>35</v>
@@ -2021,16 +2293,22 @@
         <v>35</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>149</v>
+        <v>35</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="35" ht="NA" customHeight="1">
@@ -2044,7 +2322,7 @@
         <v>35</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>35</v>
@@ -2053,16 +2331,22 @@
         <v>35</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>150</v>
+        <v>35</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="36" ht="NA" customHeight="1">
@@ -2076,7 +2360,7 @@
         <v>35</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>35</v>
@@ -2085,16 +2369,22 @@
         <v>35</v>
       </c>
       <c r="G36" s="7" t="n">
-        <v>-0.05801</v>
+        <v>-0.058</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J36" s="7" t="n">
-        <v>-0.09626</v>
+        <v>35</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" s="7" t="n">
+        <v>0.0052</v>
+      </c>
+      <c r="L36" s="7" t="n">
+        <v>-0.057</v>
       </c>
     </row>
     <row r="37" ht="NA" customHeight="1">
@@ -2108,7 +2398,7 @@
         <v>35</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>35</v>
@@ -2117,16 +2407,22 @@
         <v>35</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>151</v>
+        <v>35</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="38" ht="NA" customHeight="1">
@@ -2140,7 +2436,7 @@
         <v>35</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>35</v>
@@ -2149,16 +2445,22 @@
         <v>35</v>
       </c>
       <c r="G38" s="7" t="n">
-        <v>-0.09131</v>
+        <v>-0.091</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J38" s="7" t="n">
-        <v>-0.08396</v>
+        <v>35</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" s="7" t="n">
+        <v>-0.077</v>
+      </c>
+      <c r="L38" s="7" t="n">
+        <v>-0.067</v>
       </c>
     </row>
     <row r="39" ht="NA" customHeight="1">
@@ -2172,7 +2474,7 @@
         <v>35</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>35</v>
@@ -2181,16 +2483,22 @@
         <v>35</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>152</v>
+        <v>35</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="40" ht="NA" customHeight="1">
@@ -2204,7 +2512,7 @@
         <v>35</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>35</v>
@@ -2213,16 +2521,22 @@
         <v>35</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>153</v>
+        <v>35</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="41" ht="NA" customHeight="1">
@@ -2236,7 +2550,7 @@
         <v>35</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>35</v>
@@ -2245,16 +2559,22 @@
         <v>35</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>154</v>
+        <v>35</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="42" ht="NA" customHeight="1">
@@ -2268,7 +2588,7 @@
         <v>35</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>35</v>
@@ -2277,16 +2597,22 @@
         <v>35</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I42" s="7" t="n">
-        <v>0.00712</v>
-      </c>
-      <c r="J42" s="7" t="n">
-        <v>-0.01823</v>
+        <v>0.007</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L42" s="7" t="n">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="43" ht="NA" customHeight="1">
@@ -2300,7 +2626,7 @@
         <v>35</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>35</v>
@@ -2309,16 +2635,22 @@
         <v>35</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>155</v>
+        <v>35</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="44" ht="NA" customHeight="1">
@@ -2332,7 +2664,7 @@
         <v>35</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>35</v>
@@ -2341,16 +2673,22 @@
         <v>35</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>156</v>
+        <v>35</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="45" ht="NA" customHeight="1">
@@ -2364,7 +2702,7 @@
         <v>35</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>35</v>
@@ -2373,16 +2711,22 @@
         <v>35</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>157</v>
+        <v>35</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="46" ht="NA" customHeight="1">
@@ -2411,10 +2755,16 @@
         <v>7611</v>
       </c>
       <c r="I46" s="6" t="n">
-        <v>6786</v>
+        <v>7611</v>
       </c>
       <c r="J46" s="6" t="n">
-        <v>6785</v>
+        <v>7611</v>
+      </c>
+      <c r="K46" s="6" t="n">
+        <v>7610</v>
+      </c>
+      <c r="L46" s="6" t="n">
+        <v>7610</v>
       </c>
     </row>
     <row r="47" ht="NA" customHeight="1">
@@ -2422,31 +2772,37 @@
         <v>24</v>
       </c>
       <c r="B47" s="9" t="n">
-        <v>0.01198</v>
+        <v>0.012</v>
       </c>
       <c r="C47" s="9" t="n">
-        <v>0.03525</v>
+        <v>0.035</v>
       </c>
       <c r="D47" s="9" t="n">
-        <v>0.03313</v>
+        <v>0.033</v>
       </c>
       <c r="E47" s="9" t="n">
-        <v>0.02032</v>
+        <v>0.02</v>
       </c>
       <c r="F47" s="9" t="n">
-        <v>0.02565</v>
+        <v>0.026</v>
       </c>
       <c r="G47" s="9" t="n">
-        <v>0.05343</v>
+        <v>0.053</v>
       </c>
       <c r="H47" s="9" t="n">
-        <v>0.06469</v>
+        <v>0.065</v>
       </c>
       <c r="I47" s="9" t="n">
-        <v>0.03843</v>
+        <v>0.04</v>
       </c>
       <c r="J47" s="9" t="n">
-        <v>0.1536</v>
+        <v>0.037</v>
+      </c>
+      <c r="K47" s="9" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="L47" s="9" t="n">
+        <v>0.16</v>
       </c>
     </row>
     <row r="48" ht="NA" customHeight="1">
@@ -2480,10 +2836,16 @@
       <c r="J48" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="K48" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A48:L48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
manually fix merge issues
</commit_message>
<xml_diff>
--- a/OUTPUT/DATA/Regression output REGIONS 2022.xlsx
+++ b/OUTPUT/DATA/Regression output REGIONS 2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -74,10 +74,13 @@
     <t xml:space="preserve">RELIG11_labelAny Other Religion</t>
   </si>
   <si>
-    <t xml:space="preserve">DISEA_labelEquality Act Disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num_children</t>
+    <t xml:space="preserve">disabilityDisabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_children2 children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_children3+ children</t>
   </si>
   <si>
     <t xml:space="preserve">lev_quals_labelDegree or Equivalent</t>
@@ -110,436 +113,556 @@
     <t xml:space="preserve">Main simple (**)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.778 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.00576)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0848 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0183)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0288)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.156 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0301)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">         </t>
+    <t xml:space="preserve">0.78 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.77, 0.79]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.097 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.13, -0.066]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.06 *   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.012]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.21, -0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
   </si>
   <si>
     <t xml:space="preserve">** + age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.71 ***  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0123)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0958 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.018)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0289)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.153 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0296)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.663 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0369)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.18 ***  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0533)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.108 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0138)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0826 ***</t>
+    <t xml:space="preserve">0.71 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.69, 0.73]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.078]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.099, -0.001]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.66 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.73, -0.59]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.2 ***  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.3, -0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.085, 0.13]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.083 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.053, 0.11]    </t>
   </si>
   <si>
     <t xml:space="preserve">** + eth</t>
   </si>
   <si>
-    <t xml:space="preserve">0.798 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.00596) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0416 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.019)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0276)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.101 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0302)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.165 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0165)  </t>
+    <t xml:space="preserve">0.8 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.79, 0.81]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.043 * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.074, -0.012]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.081, 0.011]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.15, -0.053]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.17 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.19, -0.14]   </t>
   </si>
   <si>
     <t xml:space="preserve">** + child age</t>
   </si>
   <si>
-    <t xml:space="preserve">0.808 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.00659)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0824 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.15 ***  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0299)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0786 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0804 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0167)   </t>
+    <t xml:space="preserve">0.81 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.8, 0.82]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.095 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.13, -0.064]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.0085]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.15 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.2, -0.1]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.08 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.056]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.081 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.053]   </t>
   </si>
   <si>
     <t xml:space="preserve">** + famtype</t>
   </si>
   <si>
-    <t xml:space="preserve">0.674 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0131)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0877 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0182)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0287)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.149 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0298)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.13 ***  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0141)   </t>
+    <t xml:space="preserve">0.68 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.66, 0.7]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.098 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.13, -0.067]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.0057]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.12 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.1, 0.15]    </t>
   </si>
   <si>
     <t xml:space="preserve">** + religion</t>
   </si>
   <si>
-    <t xml:space="preserve">0.792 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.00817) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0459 * </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0187)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.027)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0985 **</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0303)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0113)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.162 *  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0733)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0398)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0666)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.328 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0273)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0696)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0511)  </t>
+    <t xml:space="preserve">0.79 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.78, 0.81]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.046 * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.077, -0.015]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.061, 0.028]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.099 **</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.15, -0.049]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.012, 0.026]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.28, -0.042]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.095, 0.036]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.035, 0.18]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.33 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.37, -0.28]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.17, 0.056]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.18, -0.0073] </t>
   </si>
   <si>
     <t xml:space="preserve">** + disability</t>
   </si>
   <si>
-    <t xml:space="preserve">0.832 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.00589)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0969 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0274)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.249 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0145)   </t>
+    <t xml:space="preserve">0.83 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.82, 0.84]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.078]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.092, -0.00023]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.21, -0.11]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.24 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.27, -0.22]   </t>
   </si>
   <si>
     <t xml:space="preserve">** + num_children</t>
   </si>
   <si>
-    <t xml:space="preserve">0.881 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0108)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0819 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0178)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0281)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.14 ***  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0291)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.067 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0063)   </t>
+    <t xml:space="preserve">0.8 ***  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.79, 0.82]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.093 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.12, -0.062]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.0061]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.14 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.18, -0.089]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.012, 0.026]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.23, -0.17]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">** + age + child age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.73 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.71, 0.76]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.076]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.099, -0.0011]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.29, -0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.095 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.069, 0.12]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06 **  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.025, 0.094]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.051, 0.0032]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.05 **  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.079, -0.021]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">** + eth + religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.79 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.78, 0.81]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.066, -0.0035]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.057, 0.031]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.087 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.037]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.073 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, -0.038]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.0056, 0.032]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.22, 0.023]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.037, 0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.032, 0.18]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.27 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.32, -0.22]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, 0.12]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.16, 0.0066]  </t>
   </si>
   <si>
     <t xml:space="preserve">** + lev_quals</t>
   </si>
   <si>
-    <t xml:space="preserve">0.399 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0263)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0983 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0177)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0255)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.12 ***  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.028)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.478 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0268)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.387 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0329)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.391 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.283 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.265 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0355)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.338 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0491)   </t>
+    <t xml:space="preserve">0.4 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.36, 0.45]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, -0.079]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.075, 0.011]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.12 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.17, -0.077]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.43, 0.52]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.38 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.33, 0.44]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.39 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.34, 0.44]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.23, 0.33]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.2, 0.32]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.34 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.26, 0.43]   </t>
   </si>
   <si>
     <t xml:space="preserve">full</t>
   </si>
   <si>
-    <t xml:space="preserve">0.583 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0324)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0611 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0176)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0231)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.589 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.108)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.147 **  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0515)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.079 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0133)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0181)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0699 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.02)     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0591 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0106)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.151 *   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0707)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.042)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0518)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.225 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0314)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0735)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0449)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.201 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0143)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0669 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.00643)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.354 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0277)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.273 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.033)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.294 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0292)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.218 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0297)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.257 *** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.048)    </t>
+    <t xml:space="preserve">0.51 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.46, 0.56]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.063 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.092, -0.033]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.01, 0.067]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.09, -0.0023]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.58 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.76, -0.41]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 **  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.25, -0.075]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.088 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.066, 0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.041 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.013, 0.069]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.069 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.1, -0.036]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.051 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.028, 0.074]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.033, 0.0025]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.16 *   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.27, -0.043]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.13, 0.0097]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.052, 0.11]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.22 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.27, -0.17]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.18, 0.056]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.15, 0.00051] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.22, -0.18]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.026 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.044, -0.008]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.17 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.2, -0.14]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.35 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.3, 0.39]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.27 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.22, 0.33]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3 ***  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.25, 0.34]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.22 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.17, 0.27]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.16, 0.28]    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26 *** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.18, 0.34]    </t>
   </si>
 </sst>
 </file>
@@ -998,6 +1121,8 @@
     <col min="9" max="9" width="10.71" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="10.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="10.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="10.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="10.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="NA" customHeight="1">
@@ -1005,34 +1130,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>137</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -1040,34 +1171,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>138</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
@@ -1075,34 +1212,40 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>139</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" ht="NA" customHeight="1">
@@ -1110,34 +1253,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>140</v>
+        <v>45</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>-0.035</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
@@ -1145,69 +1294,81 @@
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="n">
-        <v>-0.0518</v>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>-0.0411</v>
+        <v>-0.05</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>-0.0317</v>
+        <v>-0.035</v>
       </c>
       <c r="E6" s="7" t="n">
-        <v>-0.0481</v>
+        <v>-0.057</v>
       </c>
       <c r="F6" s="7" t="n">
-        <v>-0.0457</v>
+        <v>-0.054</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>-0.0169</v>
+        <v>-0.017</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>-0.0393</v>
+        <v>-0.046</v>
       </c>
       <c r="I6" s="7" t="n">
-        <v>-0.0463</v>
+        <v>-0.053</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>-0.0257</v>
+        <v>-0.05</v>
       </c>
       <c r="K6" s="7" t="n">
-        <v>0.0269</v>
+        <v>-0.013</v>
+      </c>
+      <c r="L6" s="7" t="n">
+        <v>-0.032</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <v>0.028</v>
       </c>
     </row>
     <row r="7" ht="NA" customHeight="1">
@@ -1215,34 +1376,40 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
@@ -1250,34 +1417,40 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="K8" s="7" t="n">
-        <v>-0.0454</v>
+        <v>73</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="M8" s="7" t="n">
+        <v>-0.046</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -1285,34 +1458,40 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>128</v>
+        <v>143</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
@@ -1320,34 +1499,40 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>143</v>
+        <v>41</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -1355,34 +1540,40 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>144</v>
+        <v>41</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
@@ -1390,34 +1581,40 @@
         <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>145</v>
+        <v>41</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
@@ -1425,34 +1622,40 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>146</v>
+        <v>41</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -1460,34 +1663,40 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>147</v>
+        <v>41</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
@@ -1495,34 +1704,40 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>148</v>
+        <v>41</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1530,34 +1745,40 @@
         <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="7" t="n">
-        <v>-0.00293</v>
+        <v>132</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="17" ht="NA" customHeight="1">
@@ -1565,34 +1786,40 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>39</v>
+        <v>133</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>149</v>
+        <v>41</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="18" ht="NA" customHeight="1">
@@ -1600,34 +1827,40 @@
         <v>9</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="19" ht="NA" customHeight="1">
@@ -1635,34 +1868,40 @@
         <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="20" ht="NA" customHeight="1">
@@ -1670,34 +1909,40 @@
         <v>10</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="J20" s="7" t="n">
+        <v>-0.024</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" ht="NA" customHeight="1">
@@ -1705,34 +1950,40 @@
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
@@ -1740,34 +1991,40 @@
         <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
@@ -1775,34 +2032,40 @@
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
@@ -1810,34 +2073,40 @@
         <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>152</v>
+        <v>41</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="25" ht="NA" customHeight="1">
@@ -1845,34 +2114,40 @@
         <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="26" ht="NA" customHeight="1">
@@ -1880,34 +2155,40 @@
         <v>13</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>0.00702</v>
+        <v>0.007</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K26" s="7" t="n">
-        <v>-0.0184</v>
+        <v>0.013</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M26" s="7" t="n">
+        <v>-0.015</v>
       </c>
     </row>
     <row r="27" ht="NA" customHeight="1">
@@ -1915,34 +2196,40 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>153</v>
+        <v>146</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="28" ht="NA" customHeight="1">
@@ -1950,34 +2237,40 @@
         <v>14</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>154</v>
+        <v>41</v>
+      </c>
+      <c r="K28" s="7" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
@@ -1985,34 +2278,40 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="30" ht="NA" customHeight="1">
@@ -2020,34 +2319,40 @@
         <v>15</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G30" s="7" t="n">
-        <v>-0.0295</v>
+        <v>-0.029</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K30" s="7" t="n">
-        <v>-0.0575</v>
+        <v>0.036</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M30" s="7" t="n">
+        <v>-0.059</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
@@ -2055,34 +2360,40 @@
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
@@ -2090,34 +2401,40 @@
         <v>16</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G32" s="7" t="n">
-        <v>0.0747</v>
+        <v>0.075</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K32" s="7" t="n">
-        <v>0.0507</v>
+        <v>0.073</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M32" s="7" t="n">
+        <v>0.031</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
@@ -2125,34 +2442,40 @@
         <v>0</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">
@@ -2160,34 +2483,40 @@
         <v>17</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="35" ht="NA" customHeight="1">
@@ -2195,34 +2524,40 @@
         <v>0</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="36" ht="NA" customHeight="1">
@@ -2230,34 +2565,40 @@
         <v>18</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G36" s="7" t="n">
         <v>-0.058</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K36" s="7" t="n">
-        <v>-0.0658</v>
+        <v>0.0052</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M36" s="7" t="n">
+        <v>-0.063</v>
       </c>
     </row>
     <row r="37" ht="NA" customHeight="1">
@@ -2265,34 +2606,40 @@
         <v>0</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="38" ht="NA" customHeight="1">
@@ -2300,34 +2647,40 @@
         <v>19</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G38" s="7" t="n">
-        <v>-0.0913</v>
+        <v>-0.091</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K38" s="7" t="n">
-        <v>-0.0787</v>
+        <v>-0.077</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M38" s="7" t="n">
+        <v>-0.073</v>
       </c>
     </row>
     <row r="39" ht="NA" customHeight="1">
@@ -2335,34 +2688,40 @@
         <v>0</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="40" ht="NA" customHeight="1">
@@ -2370,34 +2729,40 @@
         <v>20</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>162</v>
+        <v>41</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="41" ht="NA" customHeight="1">
@@ -2405,34 +2770,40 @@
         <v>0</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>163</v>
+        <v>41</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="42" ht="NA" customHeight="1">
@@ -2440,34 +2811,40 @@
         <v>21</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>117</v>
+        <v>64</v>
+      </c>
+      <c r="I42" s="7" t="n">
+        <v>0.007</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>164</v>
+        <v>41</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="43" ht="NA" customHeight="1">
@@ -2475,34 +2852,40 @@
         <v>0</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>165</v>
+        <v>41</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="44" ht="NA" customHeight="1">
@@ -2510,34 +2893,40 @@
         <v>22</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>166</v>
+        <v>41</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="45" ht="NA" customHeight="1">
@@ -2545,34 +2934,40 @@
         <v>0</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>167</v>
+        <v>41</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="46" ht="NA" customHeight="1">
@@ -2580,34 +2975,40 @@
         <v>23</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>168</v>
+        <v>41</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="47" ht="NA" customHeight="1">
@@ -2615,34 +3016,40 @@
         <v>0</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>169</v>
+        <v>41</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="48" ht="NA" customHeight="1">
@@ -2650,34 +3057,40 @@
         <v>24</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>131</v>
+        <v>41</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>170</v>
+        <v>41</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="49" ht="NA" customHeight="1">
@@ -2685,34 +3098,40 @@
         <v>0</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>171</v>
+        <v>41</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="50" ht="NA" customHeight="1">
@@ -2720,34 +3139,40 @@
         <v>25</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>172</v>
+        <v>41</v>
+      </c>
+      <c r="L50" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="51" ht="NA" customHeight="1">
@@ -2755,34 +3180,40 @@
         <v>0</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>173</v>
+        <v>41</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="52" ht="NA" customHeight="1">
@@ -2790,34 +3221,40 @@
         <v>26</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>133</v>
+        <v>41</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>172</v>
+        <v>41</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="53" ht="NA" customHeight="1">
@@ -2825,34 +3262,40 @@
         <v>0</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>134</v>
+        <v>41</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>134</v>
+        <v>41</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="54" ht="NA" customHeight="1">
@@ -2860,179 +3303,291 @@
         <v>27</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>135</v>
+        <v>41</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>174</v>
+        <v>41</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="55" ht="NA" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I55" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J55" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="K55" s="8" t="s">
-        <v>175</v>
+      <c r="B55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L55" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="56" ht="NA" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="6" t="n">
-        <v>8685</v>
-      </c>
-      <c r="C56" s="6" t="n">
-        <v>8685</v>
-      </c>
-      <c r="D56" s="6" t="n">
-        <v>8468</v>
-      </c>
-      <c r="E56" s="6" t="n">
-        <v>8685</v>
-      </c>
-      <c r="F56" s="6" t="n">
-        <v>8685</v>
-      </c>
-      <c r="G56" s="6" t="n">
+      <c r="B56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="57" ht="NA" customHeight="1">
+      <c r="A57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="M57" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" ht="NA" customHeight="1">
+      <c r="A58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="6" t="n">
         <v>7611</v>
       </c>
-      <c r="H56" s="6" t="n">
-        <v>8626</v>
-      </c>
-      <c r="I56" s="6" t="n">
-        <v>8685</v>
-      </c>
-      <c r="J56" s="6" t="n">
-        <v>8624</v>
-      </c>
-      <c r="K56" s="6" t="n">
-        <v>7517</v>
-      </c>
-    </row>
-    <row r="57" ht="NA" customHeight="1">
-      <c r="A57" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="9" t="n">
-        <v>0.0101</v>
-      </c>
-      <c r="C57" s="9" t="n">
-        <v>0.0316</v>
-      </c>
-      <c r="D57" s="9" t="n">
-        <v>0.0323</v>
-      </c>
-      <c r="E57" s="9" t="n">
-        <v>0.0182</v>
-      </c>
-      <c r="F57" s="9" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="G57" s="9" t="n">
-        <v>0.0534</v>
-      </c>
-      <c r="H57" s="9" t="n">
-        <v>0.0649</v>
-      </c>
-      <c r="I57" s="9" t="n">
-        <v>0.0309</v>
-      </c>
-      <c r="J57" s="9" t="n">
-        <v>0.0912</v>
-      </c>
-      <c r="K57" s="9" t="n">
-        <v>0.193</v>
-      </c>
-    </row>
-    <row r="58" ht="NA" customHeight="1">
-      <c r="A58" s="4" t="s">
+      <c r="C58" s="6" t="n">
+        <v>7611</v>
+      </c>
+      <c r="D58" s="6" t="n">
+        <v>7610</v>
+      </c>
+      <c r="E58" s="6" t="n">
+        <v>7611</v>
+      </c>
+      <c r="F58" s="6" t="n">
+        <v>7611</v>
+      </c>
+      <c r="G58" s="6" t="n">
+        <v>7611</v>
+      </c>
+      <c r="H58" s="6" t="n">
+        <v>7611</v>
+      </c>
+      <c r="I58" s="6" t="n">
+        <v>7611</v>
+      </c>
+      <c r="J58" s="6" t="n">
+        <v>7611</v>
+      </c>
+      <c r="K58" s="6" t="n">
+        <v>7610</v>
+      </c>
+      <c r="L58" s="6" t="n">
+        <v>7559</v>
+      </c>
+      <c r="M58" s="6" t="n">
+        <v>7558</v>
+      </c>
+    </row>
+    <row r="59" ht="NA" customHeight="1">
+      <c r="A59" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>30</v>
+      <c r="B59" s="9" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C59" s="9" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="D59" s="9" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="E59" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F59" s="9" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="G59" s="9" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="H59" s="9" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="I59" s="9" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="J59" s="9" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="K59" s="9" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="L59" s="9" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="M59" s="9" t="n">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="60" ht="NA" customHeight="1">
+      <c r="A60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A60:M60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -3292,9 +3847,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E2C24D0-E859-494D-AE91-FDFD398D20B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23571F4C-ACF5-438B-8992-1F785BBB6100}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51F7D0F1-6897-4B2A-9F2D-4C066DF14374}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ECDBE70-608C-446A-9111-E9C20519953C}"/>
 </file>
</xml_diff>